<commit_message>
another run of v4
</commit_message>
<xml_diff>
--- a/Run_v2_PearsonSpearman.xlsx
+++ b/Run_v2_PearsonSpearman.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>Pearson</t>
   </si>
@@ -47,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -57,14 +57,26 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,28 +96,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>0.9749233470445906</v>
+        <v>0.98022782785691354</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.97713018829915088</v>
+        <v>0.9622607019793904</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>